<commit_message>
VERSAO = "10.36 05/06/2023"
VERSAO = "10.36 05/06/2023"
</commit_message>
<xml_diff>
--- a/ESP32.xlsx
+++ b/ESP32.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dm8-my.sharepoint.com/personal/flavio_cabral_dm8_com_br/Documents/Documentos/GitHub/Autormacao_esp32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_BC54B5FEE25CE662683F85144872501328FAE4EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D38FAE22-45A2-48C4-BA83-72ED40E8938A}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_BC54B5FEE25CE662683F85144872501328FAE4EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CBD9E3C-45EA-4393-903B-235CF29451B1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="990" yWindow="1530" windowWidth="18000" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>GND</t>
   </si>
@@ -221,17 +221,23 @@
     <t>BUZZER</t>
   </si>
   <si>
-    <t>PIR</t>
-  </si>
-  <si>
     <t>IR</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +265,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="-0.249977111117893"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,12 +294,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,12 +323,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -384,11 +390,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,38 +448,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -899,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:J18"/>
+  <dimension ref="C3:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,21 +973,21 @@
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="2">
         <v>23</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="6" t="s">
-        <v>28</v>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
@@ -934,21 +995,21 @@
       <c r="I5" s="2">
         <v>22</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C7" s="12" t="s">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2">
@@ -957,10 +1018,10 @@
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="2">
@@ -969,12 +1030,12 @@
       <c r="I8" s="2">
         <v>21</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="2">
@@ -983,12 +1044,12 @@
       <c r="I9" s="2">
         <v>19</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J9" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2">
@@ -997,12 +1058,12 @@
       <c r="I10" s="2">
         <v>18</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2">
@@ -1011,10 +1072,15 @@
       <c r="I11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="11"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+      <c r="J11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="2">
@@ -1023,12 +1089,13 @@
       <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+      <c r="J12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="14"/>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="2">
@@ -1037,10 +1104,10 @@
       <c r="I13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+      <c r="J13" s="12"/>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="2">
@@ -1049,12 +1116,12 @@
       <c r="I14" s="2">
         <v>4</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="2">
@@ -1063,12 +1130,12 @@
       <c r="I15" s="2">
         <v>2</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="2">
@@ -1077,7 +1144,7 @@
       <c r="I16" s="2">
         <v>15</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1099,6 +1166,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K11:K12"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
VERSAO = "10.37 05/06/2023"
VERSAO = "10.37 05/06/2023"
Desativando sensor EmonLib.h
</commit_message>
<xml_diff>
--- a/ESP32.xlsx
+++ b/ESP32.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dm8-my.sharepoint.com/personal/flavio_cabral_dm8_com_br/Documents/Documentos/GitHub/Autormacao_esp32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_BC54B5FEE25CE662683F85144872501328FAE4EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CBD9E3C-45EA-4393-903B-235CF29451B1}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_BC54B5FEE25CE662683F85144872501328FAE4EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2912409-A138-4F77-8F6F-374A53E1FDD2}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="1530" windowWidth="18000" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>GND</t>
   </si>
@@ -222,15 +222,6 @@
   </si>
   <si>
     <t>IR</t>
-  </si>
-  <si>
-    <t>CLK</t>
-  </si>
-  <si>
-    <t>DIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display </t>
   </si>
 </sst>
 </file>
@@ -478,16 +469,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -963,7 +954,7 @@
   <dimension ref="C3:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,12 +1063,8 @@
       <c r="I11" s="2">
         <v>5</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>30</v>
-      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C12" s="3" t="s">
@@ -1089,10 +1076,8 @@
       <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="16"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">

</xml_diff>